<commit_message>
Adição da Ata do dia 08/10/2024
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 0310/Grupo4_ATA_Semana0310.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 0310/Grupo4_ATA_Semana0310.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4fd29038e46714d/Área de Trabalho/SPTECH/Pesquisa e Inovação/Sprint-SPTECH/ATAs_de_Reuniao/Sprint 2/Semana 0310/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTech\GitHub\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 0310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{2BD8E110-567F-46BF-8156-99AF290F6DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{308D140B-E512-41E1-8818-7FF72186DB17}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7549776-5EAD-44D7-84D5-262F63A0CBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="1" activeTab="3" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sexta" sheetId="11" r:id="rId3"/>
     <sheet name="Sábado" sheetId="12" r:id="rId4"/>
     <sheet name="Segunda" sheetId="13" r:id="rId5"/>
-    <sheet name="Terça" sheetId="14" r:id="rId6"/>
+    <sheet name="Terça" sheetId="16" r:id="rId6"/>
     <sheet name="Quarta" sheetId="15" r:id="rId7"/>
     <sheet name="SEMANAL" sheetId="10" r:id="rId8"/>
   </sheets>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="69">
   <si>
     <t>NOME</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Foi apresentado o trabalho feito no final de semana por cada integrante do grupo e decidido como seria o novo protótipo do Site. Também definimos pontos acerca das tabelas que farão parte do banco de dados.</t>
   </si>
   <si>
-    <t>Foi discutido sobre o prazo da entrega das atividades, falado sobre o mySQL na VM local e por ultimo também realizamos um teste para a apresentação sobre a metodologia PERT</t>
-  </si>
-  <si>
     <t>Foi discutido sobre o prazo da entrega das atividades, falado sobre as tabelas e sua modelação no MySQL, atualização do Backlog e os próximos passos para o projeto.</t>
   </si>
   <si>
@@ -247,14 +244,21 @@
   </si>
   <si>
     <t>Finalizamos o backlog do projeto acrescentando as tarefas faltantes e os responsáveis por cada demanda. Também definimos o restante das tabelas de bando de dados que serão utilizadas na Sprint 2.</t>
+  </si>
+  <si>
+    <t>Foi reorganizado os prazos de entrega das tarefas, debatido sobre as mudanças que irão ocorrer no grupo por conta da perda de um integrante, além disso falamos sobre o feedback que recebemos com a reunião com o Marcos.</t>
+  </si>
+  <si>
+    <t>Trancou o curso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -774,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -931,6 +935,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -958,62 +1013,15 @@
     <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="127">
+  <dxfs count="136">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1076,6 +1084,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1096,6 +1124,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1176,6 +1224,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1186,6 +1254,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1226,6 +1304,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1236,6 +1324,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1416,7 +1514,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1432,129 +1530,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1589,8 +1564,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1628,17 +1602,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1658,7 +1622,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1678,8 +1642,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1699,17 +1663,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1730,6 +1684,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1764,7 +1738,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1784,12 +1758,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1804,7 +1778,29 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1839,7 +1835,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1877,7 +1874,17 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1897,7 +1904,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1917,8 +1924,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1938,7 +1945,17 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1959,26 +1976,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2166,7 +2163,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2415,7 +2412,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2608,6 +2605,87 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FF000000"/>
@@ -2625,6 +2703,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2812,7 +2910,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3061,7 +3159,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3154,191 +3252,191 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125" tableBorderDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="132"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="131"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1191F4CB-7F6D-485B-AC60-0502347DD05B}" name="Tabela216579" displayName="Tabela216579" ref="A23:C29" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A23:C29" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" tableBorderDxfId="48">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8CE1CFB1-3B41-4ED3-8123-1F497AD0EBF4}" name="NOME" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{D65F61F3-2928-4DDE-B139-E3881CA88028}" name="PARTICIPAÇÃO" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{E75E5DBF-4EBF-4291-8B2C-1C27A0B29355}" name="JUSTIFICATIVA" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D14" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D14" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A23:C29" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A23:C29" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D17" totalsRowShown="0" headerRowDxfId="53" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D17" totalsRowShown="0" headerRowDxfId="70" tableBorderDxfId="69">
   <autoFilter ref="A7:D17" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I14" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="F7:I14" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
     <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127" tableBorderDxfId="126">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="116"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="115"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" tableBorderDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" tableBorderDxfId="120">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="107"/>
+    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="117"/>
+    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" tableBorderDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114" tableBorderDxfId="113">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="101"/>
+    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D15" totalsRowShown="0" headerRowDxfId="100" dataDxfId="36" tableBorderDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D15" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" tableBorderDxfId="107">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A24:C30" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97" tableBorderDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A24:C30" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101" tableBorderDxfId="100">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" tableBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="88"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="87"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{433F7683-AF81-4BA7-9443-5B185A6FB802}" name="Tabela115468" displayName="Tabela115468" ref="A4:D14" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" tableBorderDxfId="77">
-  <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D14" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
+  <autoFilter ref="A4:D14" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9478A723-D368-432D-B04D-0CE3A8B04818}" name="O QUE FAZER" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{299E99A9-2BDD-4259-B821-126259D6061E}" name="PRAZOS DE ENTREGA" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{885DF8C6-2582-4A91-9775-AD5DDBFE5E62}" name="RESPONSAVEL" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{653F985A-2FB8-486B-BC74-444331BCE755}" name="SITUAÇÃO" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3667,12 +3765,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3683,7 +3781,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3694,7 +3792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3712,17 +3810,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -3730,8 +3828,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -3743,7 +3841,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3761,9 +3859,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="6">
         <v>45574</v>
@@ -3779,7 +3877,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -3793,7 +3891,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -3807,9 +3905,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="6">
         <v>45574</v>
@@ -3821,9 +3919,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="6">
         <v>45574</v>
@@ -3835,9 +3933,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="6">
         <v>45574</v>
@@ -3849,9 +3947,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="6">
         <v>45574</v>
@@ -3863,9 +3961,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6">
         <v>45574</v>
@@ -3877,8 +3975,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
@@ -3886,34 +3984,34 @@
       <c r="C14" s="22"/>
       <c r="D14" s="23"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="29"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
       <c r="D16" s="32"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
       <c r="D17" s="32"/>
     </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>19</v>
       </c>
@@ -3923,7 +4021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -3937,7 +4035,7 @@
         <v>45568</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -3949,7 +4047,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -3961,7 +4059,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -3973,7 +4071,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -3985,7 +4083,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -3997,7 +4095,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -4024,21 +4122,21 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4082,17 +4180,17 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -4100,8 +4198,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -4113,7 +4211,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4131,9 +4229,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4149,7 +4247,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -4163,7 +4261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -4177,7 +4275,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -4191,7 +4289,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -4205,7 +4303,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -4219,7 +4317,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4233,9 +4331,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="6">
         <v>45572</v>
@@ -4247,7 +4345,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -4261,9 +4359,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="6">
         <v>45574</v>
@@ -4275,9 +4373,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="6">
         <v>45575</v>
@@ -4289,8 +4387,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>29</v>
       </c>
@@ -4298,34 +4396,34 @@
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
     </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
       <c r="D20" s="32"/>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
@@ -4335,7 +4433,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -4349,7 +4447,7 @@
         <v>45569</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -4361,7 +4459,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -4373,7 +4471,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -4385,7 +4483,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -4397,7 +4495,7 @@
         <v>0.69166666666666665</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -4409,7 +4507,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -4432,21 +4530,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D15">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4486,21 +4584,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25161DFF-344A-4C41-AE51-A14BEC6B2F7D}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -4508,8 +4606,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -4521,7 +4619,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4539,9 +4637,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4557,7 +4655,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -4571,7 +4669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -4585,7 +4683,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -4599,7 +4697,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -4613,7 +4711,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -4627,7 +4725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4641,9 +4739,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="6">
         <v>45572</v>
@@ -4655,7 +4753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -4669,9 +4767,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="6">
         <v>45574</v>
@@ -4683,9 +4781,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="6">
         <v>45575</v>
@@ -4697,13 +4795,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>29</v>
       </c>
@@ -4711,34 +4809,34 @@
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
     </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
       <c r="D20" s="32"/>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
@@ -4748,7 +4846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -4762,7 +4860,7 @@
         <v>45570</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -4774,7 +4872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -4786,7 +4884,7 @@
         <v>0.4236111111111111</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -4798,7 +4896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -4810,7 +4908,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -4822,7 +4920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -4845,21 +4943,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D16">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4906,17 +5004,17 @@
       <selection activeCell="B5" sqref="B5:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -4924,8 +5022,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -4937,7 +5035,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4955,7 +5053,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -4973,7 +5071,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -4987,7 +5085,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -5001,7 +5099,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -5015,7 +5113,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -5029,7 +5127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5043,7 +5141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5057,7 +5155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -5071,7 +5169,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -5085,14 +5183,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
@@ -5100,7 +5198,7 @@
       <c r="C16" s="22"/>
       <c r="D16" s="23"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>51</v>
       </c>
@@ -5108,26 +5206,26 @@
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>19</v>
       </c>
@@ -5137,7 +5235,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -5151,7 +5249,7 @@
         <v>45565</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -5163,7 +5261,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -5175,7 +5273,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -5187,7 +5285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -5199,7 +5297,7 @@
         <v>0.69513888888888886</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -5211,7 +5309,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -5234,21 +5332,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5285,24 +5383,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4588FE3E-D7A2-4335-AA32-FE123603ED1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C19D80-51B6-43B3-9932-AE225A9BF602}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="38.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -5310,8 +5408,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -5323,7 +5421,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5341,30 +5439,30 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="6">
-        <v>45569</v>
+        <v>45575</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="6">
-        <v>45568</v>
+        <v>45575</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -5373,12 +5471,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="6">
-        <v>45569</v>
+        <v>45575</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -5387,12 +5485,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="6">
-        <v>45568</v>
+        <v>45575</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
@@ -5401,26 +5499,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B9" s="6">
-        <v>45567</v>
+        <v>45572</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="6">
-        <v>45567</v>
+        <v>45575</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>9</v>
@@ -5429,40 +5527,40 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="6">
-        <v>45567</v>
+        <v>45575</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="6">
-        <v>45567</v>
+        <v>45575</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="6">
-        <v>45567</v>
+        <v>45575</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
@@ -5471,14 +5569,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="71">
+        <v>45575</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
@@ -5486,34 +5597,34 @@
       <c r="C16" s="22"/>
       <c r="D16" s="23"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>19</v>
       </c>
@@ -5523,7 +5634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -5534,10 +5645,10 @@
         <v>7</v>
       </c>
       <c r="D23" s="4">
-        <v>45566</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>45573</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -5549,7 +5660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -5558,22 +5669,24 @@
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="7">
-        <v>0.68333333333333335</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.73611111111111116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D26" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -5582,10 +5695,10 @@
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="8">
-        <v>0.69305555555555554</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.75138888888888888</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -5597,7 +5710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -5607,7 +5720,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="3">
         <f>IF(D27="","",D27-D25)</f>
-        <v>9.7222222222221877E-3</v>
+        <v>1.5277777777777724E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5620,27 +5733,41 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+  <conditionalFormatting sqref="D5:D14">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C14" xr:uid="{2915FD14-172A-47B4-A85D-63A71A474370}">
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>"Finalizada"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+      <formula>"Em Andamento"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>"Pendente"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C8 C10:C14" xr:uid="{4EF0152B-2ADC-4784-A8EB-10969926F4CD}">
       <formula1>$A$24:$A$29</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{2C3DF937-3168-405C-85F3-926E2777944E}">
+      <formula1>$A$25:$A$30</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5652,13 +5779,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F897371B-825E-46C1-AE8C-F5A30A71FAE7}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{454FC0B6-946A-4E2F-A8AD-0CB0E84B9580}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
           <xm:sqref>B24:B29</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DF141593-0456-44A9-8FC5-DB7C1738BC4E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5A9302DE-4F93-496E-A98E-9F09E6CBE775}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
@@ -5678,17 +5805,17 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -5696,8 +5823,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -5709,7 +5836,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5727,7 +5854,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -5745,7 +5872,7 @@
       <c r="H5" s="20"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -5759,7 +5886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -5773,7 +5900,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -5787,7 +5914,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -5801,7 +5928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5815,7 +5942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5829,7 +5956,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -5843,7 +5970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -5857,14 +5984,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
@@ -5872,34 +5999,34 @@
       <c r="C16" s="22"/>
       <c r="D16" s="23"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
       <c r="D18" s="41"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39"/>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
       <c r="D19" s="41"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="42"/>
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
       <c r="D20" s="44"/>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>19</v>
       </c>
@@ -5909,7 +6036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -5923,7 +6050,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -5935,7 +6062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -5947,7 +6074,7 @@
         <v>0.68194444444444446</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -5959,7 +6086,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -5971,7 +6098,7 @@
         <v>0.6958333333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -5983,7 +6110,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -6006,21 +6133,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6067,21 +6194,21 @@
       <selection activeCell="F8" sqref="F8:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.08984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="1"/>
+    <col min="7" max="7" width="31.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>40</v>
       </c>
@@ -6094,8 +6221,8 @@
       <c r="H1" s="22"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>30</v>
       </c>
@@ -6103,50 +6230,50 @@
       <c r="C3" s="22"/>
       <c r="D3" s="23"/>
       <c r="F3" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="I3" s="23"/>
     </row>
-    <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
       <c r="F4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="56"/>
-      <c r="I4" s="57"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
       <c r="F5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="58" t="s">
+      <c r="G5" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="59"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
@@ -6172,7 +6299,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>48</v>
       </c>
@@ -6186,7 +6313,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="6">
         <v>45574</v>
@@ -6198,9 +6325,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -6224,7 +6351,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>37</v>
       </c>
@@ -6250,7 +6377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>27</v>
       </c>
@@ -6264,7 +6391,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="6">
         <v>45574</v>
@@ -6276,7 +6403,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>36</v>
       </c>
@@ -6290,7 +6417,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" s="6">
         <v>45574</v>
@@ -6302,7 +6429,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>35</v>
       </c>
@@ -6316,7 +6443,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" s="6">
         <v>45574</v>
@@ -6328,7 +6455,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>34</v>
       </c>
@@ -6342,7 +6469,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G14" s="6">
         <v>45574</v>
@@ -6354,7 +6481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>49</v>
       </c>
@@ -6368,7 +6495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>38</v>
       </c>
@@ -6382,7 +6509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -6396,13 +6523,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>31</v>
       </c>
@@ -6410,120 +6537,128 @@
       <c r="C19" s="22"/>
       <c r="D19" s="23"/>
     </row>
-    <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
       <c r="D20" s="29"/>
     </row>
-    <row r="21" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
       <c r="D21" s="32"/>
       <c r="E21" s="13"/>
     </row>
-    <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
     </row>
-    <row r="23" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33"/>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
       <c r="D23" s="35"/>
     </row>
-    <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="60" t="s">
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="62"/>
-    </row>
-    <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="67" t="s">
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="68"/>
-      <c r="C26" s="63" t="s">
+      <c r="B26" s="59"/>
+      <c r="C26" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="64"/>
-    </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="69" t="s">
+      <c r="D26" s="55"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65" t="s">
+      <c r="B27" s="56"/>
+      <c r="C27" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="66"/>
-    </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="70" t="s">
+      <c r="D27" s="57"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54" t="s">
+      <c r="B28" s="45"/>
+      <c r="C28" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="55"/>
-    </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="45" t="s">
+      <c r="D28" s="46"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46" t="s">
+      <c r="B29" s="63"/>
+      <c r="C29" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="52"/>
-    </row>
-    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="47" t="s">
+      <c r="D29" s="69"/>
+    </row>
+    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48" t="s">
+      <c r="B30" s="65"/>
+      <c r="C30" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="53"/>
-    </row>
-    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="45" t="s">
+      <c r="D30" s="70"/>
+    </row>
+    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46" t="s">
+      <c r="B31" s="63"/>
+      <c r="C31" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="52"/>
-    </row>
-    <row r="32" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="49" t="s">
+      <c r="D31" s="69"/>
+    </row>
+    <row r="32" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50" t="s">
+      <c r="B32" s="67"/>
+      <c r="C32" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="51"/>
+      <c r="D32" s="68"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:D23"/>
@@ -6540,24 +6675,16 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="I8:I14 D8:D18">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Upload da ATA do dia 09/10
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 0310/Grupo4_ATA_Semana0310.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 0310/Grupo4_ATA_Semana0310.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTech\GitHub\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 0310\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\Semana 0310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7549776-5EAD-44D7-84D5-262F63A0CBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F54A0D-A5F4-4AEE-847A-2BE48897ACF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="71">
   <si>
     <t>NOME</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Foi apresentado o trabalho feito no final de semana por cada integrante do grupo e decidido como seria o novo protótipo do Site. Também definimos pontos acerca das tabelas que farão parte do banco de dados.</t>
   </si>
   <si>
-    <t>Foi discutido sobre o prazo da entrega das atividades, falado sobre as tabelas e sua modelação no MySQL, atualização do Backlog e os próximos passos para o projeto.</t>
-  </si>
-  <si>
     <t>CALCULADORA</t>
   </si>
   <si>
@@ -250,15 +247,23 @@
   </si>
   <si>
     <t>Trancou o curso</t>
+  </si>
+  <si>
+    <t>DASHBOARD ESTÁTICA</t>
+  </si>
+  <si>
+    <t>Foi discutido a respeito do banco de dados, das telas de cadastro e login e a calculadora.</t>
+  </si>
+  <si>
+    <t>Possivelmente saiu da faculdade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -778,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -899,10 +904,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -935,6 +936,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -985,43 +1013,12 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="136">
+  <dxfs count="124">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1084,6 +1081,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1094,6 +1101,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1114,6 +1131,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1124,6 +1151,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1144,6 +1181,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1154,6 +1201,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1224,6 +1281,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1234,6 +1301,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1274,206 +1351,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1489,7 +1366,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1509,12 +1386,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1529,7 +1406,29 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1564,7 +1463,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1602,7 +1502,17 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1622,7 +1532,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1642,8 +1552,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1663,7 +1573,17 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1684,26 +1604,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1738,7 +1638,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1758,12 +1658,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1778,29 +1678,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1835,8 +1713,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1874,17 +1751,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1904,7 +1771,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1924,8 +1791,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1945,17 +1812,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1976,6 +1833,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2163,7 +2040,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2412,7 +2289,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2661,7 +2538,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2910,7 +2787,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3159,7 +3036,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3252,191 +3129,191 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122" tableBorderDxfId="121">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="132"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="131"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="130"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="129"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A23:C29" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" tableBorderDxfId="48">
-  <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DF67C996-856A-46BE-858A-EE661CA1DC38}" name="Tabela2165713" displayName="Tabela2165713" ref="A22:C28" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+  <autoFilter ref="A22:C28" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{9F9FFDDA-0637-482D-BE7C-9123DF19F3C1}" name="NOME" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{3EAC496C-C984-4E87-A163-F9C5F4690901}" name="PARTICIPAÇÃO" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{6FC35D35-5B2B-461B-BA9D-4DE2632E81DC}" name="JUSTIFICATIVA" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D14" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" tableBorderDxfId="81">
-  <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
-    <sortCondition ref="B5:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D12" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
+  <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
+    <sortCondition ref="B5:B12"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A23:C29" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
-  <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A21:C27" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49">
+  <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D17" totalsRowShown="0" headerRowDxfId="70" tableBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D17" totalsRowShown="0" headerRowDxfId="45" tableBorderDxfId="44">
   <autoFilter ref="A7:D17" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I14" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I14" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
   <autoFilter ref="F7:I14" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
     <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127" tableBorderDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" tableBorderDxfId="114">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="125"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="124"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="123"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" tableBorderDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" tableBorderDxfId="108">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="117"/>
-    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="116"/>
+    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="106"/>
+    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="105"/>
+    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114" tableBorderDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102" tableBorderDxfId="101">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="111"/>
-    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D15" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" tableBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D15" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96" tableBorderDxfId="95">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="103"/>
+    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A24:C30" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101" tableBorderDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A24:C30" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D14" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
-  <autoFilter ref="A4:D14" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
-    <sortCondition ref="B5:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}" name="Tabela1154612" displayName="Tabela1154612" ref="A4:D13" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" tableBorderDxfId="69">
+  <autoFilter ref="A4:D13" xr:uid="{8B87E3DE-020E-4DB1-B973-FEA4CF144636}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D13">
+    <sortCondition ref="B5:B13"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{4CD68898-BF51-40F7-8A2C-0ED0A2C43325}" name="O QUE FAZER" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{D549D94A-6AE3-4343-A22F-FA226F905EFD}" name="PRAZOS DE ENTREGA" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{7C74E9E5-8939-4A73-B489-AE85EF3FBCBF}" name="RESPONSAVEL" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{42898429-7E82-4C5F-9E36-A0417F741348}" name="SITUAÇÃO" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3765,12 +3642,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3781,7 +3658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3792,7 +3669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3810,17 +3687,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="37.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -3828,8 +3705,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -3841,7 +3718,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3859,9 +3736,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="6">
         <v>45574</v>
@@ -3877,7 +3754,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -3891,7 +3768,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -3905,9 +3782,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="6">
         <v>45574</v>
@@ -3919,9 +3796,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="6">
         <v>45574</v>
@@ -3933,9 +3810,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="6">
         <v>45574</v>
@@ -3947,9 +3824,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="6">
         <v>45574</v>
@@ -3961,9 +3838,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="6">
         <v>45574</v>
@@ -3975,8 +3852,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
@@ -3984,34 +3861,34 @@
       <c r="C14" s="22"/>
       <c r="D14" s="23"/>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="29"/>
     </row>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="30"/>
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
       <c r="D16" s="32"/>
     </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="30"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
       <c r="D17" s="32"/>
     </row>
-    <row r="18" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="33"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="24" t="s">
         <v>19</v>
       </c>
@@ -4021,7 +3898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4035,7 +3912,7 @@
         <v>45568</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4047,7 +3924,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4059,7 +3936,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -4071,7 +3948,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -4083,7 +3960,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -4095,7 +3972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -4122,21 +3999,21 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B22:B27">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4180,17 +4057,17 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -4198,8 +4075,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -4211,7 +4088,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4229,9 +4106,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4247,7 +4124,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -4261,7 +4138,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -4275,7 +4152,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -4289,7 +4166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -4303,7 +4180,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -4317,7 +4194,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4331,9 +4208,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="6">
         <v>45572</v>
@@ -4345,7 +4222,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -4359,9 +4236,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="6">
         <v>45574</v>
@@ -4373,9 +4250,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="6">
         <v>45575</v>
@@ -4387,8 +4264,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:4" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21" t="s">
         <v>29</v>
       </c>
@@ -4396,34 +4273,34 @@
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
     </row>
-    <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="30"/>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="30"/>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
       <c r="D20" s="32"/>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="33"/>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
@@ -4433,7 +4310,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -4447,7 +4324,7 @@
         <v>45569</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -4459,7 +4336,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -4471,7 +4348,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -4483,7 +4360,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -4495,7 +4372,7 @@
         <v>0.69166666666666665</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -4507,7 +4384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -4530,21 +4407,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D15">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4588,17 +4465,17 @@
       <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -4606,8 +4483,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -4619,7 +4496,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4637,9 +4514,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4655,7 +4532,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -4669,7 +4546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -4683,7 +4560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -4697,7 +4574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -4711,7 +4588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -4725,7 +4602,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4739,9 +4616,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="6">
         <v>45572</v>
@@ -4753,7 +4630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -4767,9 +4644,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="6">
         <v>45574</v>
@@ -4781,9 +4658,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="6">
         <v>45575</v>
@@ -4795,13 +4672,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="21" t="s">
         <v>29</v>
       </c>
@@ -4809,34 +4686,34 @@
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
     </row>
-    <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="30"/>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="30"/>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
       <c r="D20" s="32"/>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="33"/>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
@@ -4846,7 +4723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -4860,7 +4737,7 @@
         <v>45570</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -4872,7 +4749,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -4884,7 +4761,7 @@
         <v>0.4236111111111111</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -4896,7 +4773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -4908,7 +4785,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -4920,7 +4797,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -4943,21 +4820,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="34" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D16">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5004,17 +4881,17 @@
       <selection activeCell="B5" sqref="B5:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -5022,8 +4899,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -5035,7 +4912,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5053,7 +4930,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -5071,7 +4948,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -5085,7 +4962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -5099,7 +4976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -5113,7 +4990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -5127,7 +5004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5141,7 +5018,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5155,7 +5032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -5169,7 +5046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -5183,14 +5060,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:9" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
@@ -5198,7 +5075,7 @@
       <c r="C16" s="22"/>
       <c r="D16" s="23"/>
     </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27" t="s">
         <v>51</v>
       </c>
@@ -5206,26 +5083,26 @@
       <c r="C17" s="28"/>
       <c r="D17" s="29"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="30"/>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="30"/>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="24" t="s">
         <v>19</v>
       </c>
@@ -5235,7 +5112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -5249,7 +5126,7 @@
         <v>45565</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -5261,7 +5138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -5273,7 +5150,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -5285,7 +5162,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -5297,7 +5174,7 @@
         <v>0.69513888888888886</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -5309,7 +5186,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -5332,21 +5209,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5384,23 +5261,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C19D80-51B6-43B3-9932-AE225A9BF602}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="38.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -5408,8 +5285,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -5421,7 +5298,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5439,7 +5316,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -5457,7 +5334,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -5471,7 +5348,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -5485,7 +5362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -5499,9 +5376,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="6">
         <v>45572</v>
@@ -5513,7 +5390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5527,7 +5404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5541,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -5555,7 +5432,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -5566,160 +5443,146 @@
         <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="71">
-        <v>45575</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-    </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
+    </row>
+    <row r="17" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="30"/>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
-    </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+    <row r="19" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="12" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+    <row r="22" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D22" s="4">
         <v>45573</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="7">
+        <v>0.73611111111111116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="7">
-        <v>0.73611111111111116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="5"/>
+      <c r="D26" s="8">
+        <v>0.75138888888888888</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="8">
-        <v>0.75138888888888888</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="3">
-        <f>IF(D27="","",D27-D25)</f>
+      <c r="D28" s="3">
+        <f>IF(D26="","",D26-D24)</f>
         <v>1.5277777777777724E-2</v>
       </c>
     </row>
@@ -5728,46 +5591,35 @@
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D20"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D19"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
-  <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
+  <conditionalFormatting sqref="B23:B28">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D14">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+  <conditionalFormatting sqref="D5:D13">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
-      <formula>"Pendente"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
-      <formula>"Finalizada"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
-      <formula>"Em Andamento"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C8 C10:C14" xr:uid="{4EF0152B-2ADC-4784-A8EB-10969926F4CD}">
-      <formula1>$A$24:$A$29</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C8 C10:C13" xr:uid="{4EF0152B-2ADC-4784-A8EB-10969926F4CD}">
+      <formula1>$A$23:$A$28</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{2C3DF937-3168-405C-85F3-926E2777944E}">
-      <formula1>$A$25:$A$30</formula1>
+      <formula1>$A$24:$A$29</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5783,13 +5635,13 @@
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B24:B29</xm:sqref>
+          <xm:sqref>B23:B28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5A9302DE-4F93-496E-A98E-9F09E6CBE775}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D14</xm:sqref>
+          <xm:sqref>D5:D13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5799,23 +5651,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA814AF-35E5-4596-923E-E8BF36EBF589}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
@@ -5823,8 +5675,8 @@
       <c r="C1" s="22"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
@@ -5836,7 +5688,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5854,30 +5706,30 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="6">
-        <v>45569</v>
+        <v>45575</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5" s="20"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B6" s="6">
-        <v>45568</v>
+        <v>45575</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -5886,26 +5738,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B7" s="6">
-        <v>45569</v>
+        <v>45575</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B8" s="6">
-        <v>45568</v>
+        <v>45572</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
@@ -5914,213 +5766,195 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B9" s="6">
-        <v>45567</v>
+        <v>45575</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45575</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45567</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B11" s="6">
-        <v>45567</v>
+        <v>45575</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B12" s="6">
-        <v>45567</v>
+        <v>45575</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="6">
-        <v>45567</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+    <row r="13" spans="1:9" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:9" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38"/>
-    </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="44"/>
-    </row>
-    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+    </row>
+    <row r="16" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
+    </row>
+    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+    </row>
+    <row r="18" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="43"/>
+    </row>
+    <row r="19" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4">
+        <v>45574</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="4">
-        <v>45567</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7">
+        <v>0.68194444444444446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="D24" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="7">
-        <v>0.68194444444444446</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="8">
+        <v>0.7055555555555556</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="8">
-        <v>0.6958333333333333</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="3">
-        <f>IF(D27="","",D27-D25)</f>
-        <v>1.388888888888884E-2</v>
+      <c r="D27" s="3">
+        <f>IF(D25="","",D25-D23)</f>
+        <v>2.3611111111111138E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6128,36 +5962,42 @@
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D20"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D18"/>
+    <mergeCell ref="A20:C20"/>
   </mergeCells>
-  <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+  <conditionalFormatting sqref="B22:B27">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+  <conditionalFormatting sqref="D5:D12">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C14" xr:uid="{95397FFA-5041-4E31-8F3C-B8B001CC0655}">
-      <formula1>$A$24:$A$29</formula1>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12 C8" xr:uid="{95397FFA-5041-4E31-8F3C-B8B001CC0655}">
+      <formula1>$A$22:$A$27</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C11 C5:C7" xr:uid="{BF6BE469-1BEA-4523-8665-4CADFDE409AC}">
+      <formula1>$A$21:$A$26</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C7" listDataValidation="1"/>
+  </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -6165,17 +6005,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B7FF22DE-2014-4A18-A8C0-5CF4DEDDE2F2}">
+          <x14:formula1>
+            <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B22:B27</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E0636FB-9A1D-4159-B803-CA79D507499D}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D14</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B7FF22DE-2014-4A18-A8C0-5CF4DEDDE2F2}">
-          <x14:formula1>
-            <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>B24:B29</xm:sqref>
+          <xm:sqref>D5:D12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6194,21 +6034,21 @@
       <selection activeCell="F8" sqref="F8:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="31.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>40</v>
       </c>
@@ -6221,8 +6061,8 @@
       <c r="H1" s="22"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="21" t="s">
         <v>30</v>
       </c>
@@ -6230,50 +6070,50 @@
       <c r="C3" s="22"/>
       <c r="D3" s="23"/>
       <c r="F3" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="I3" s="23"/>
     </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="56"/>
       <c r="F4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="55"/>
+      <c r="I4" s="56"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
       <c r="F5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="57"/>
+      <c r="I5" s="58"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
@@ -6299,7 +6139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>48</v>
       </c>
@@ -6313,7 +6153,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="6">
         <v>45574</v>
@@ -6325,9 +6165,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -6351,7 +6191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>37</v>
       </c>
@@ -6377,7 +6217,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>27</v>
       </c>
@@ -6391,7 +6231,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="6">
         <v>45574</v>
@@ -6403,7 +6243,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>36</v>
       </c>
@@ -6417,7 +6257,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="6">
         <v>45574</v>
@@ -6429,7 +6269,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>35</v>
       </c>
@@ -6443,7 +6283,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="6">
         <v>45574</v>
@@ -6455,7 +6295,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>34</v>
       </c>
@@ -6469,7 +6309,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="6">
         <v>45574</v>
@@ -6481,7 +6321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>49</v>
       </c>
@@ -6495,7 +6335,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>38</v>
       </c>
@@ -6509,7 +6349,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -6523,13 +6363,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="21" t="s">
         <v>31</v>
       </c>
@@ -6537,128 +6377,120 @@
       <c r="C19" s="22"/>
       <c r="D19" s="23"/>
     </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
       <c r="D20" s="29"/>
     </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="30"/>
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
       <c r="D21" s="32"/>
       <c r="E21" s="13"/>
     </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="30"/>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
     </row>
-    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="33"/>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
       <c r="D23" s="35"/>
     </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51" t="s">
+    <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="53"/>
-    </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="58" t="s">
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="61"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="59"/>
-      <c r="C26" s="54" t="s">
+      <c r="B26" s="67"/>
+      <c r="C26" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="55"/>
-    </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
+      <c r="D26" s="63"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56" t="s">
+      <c r="B27" s="64"/>
+      <c r="C27" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="57"/>
-    </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
+      <c r="D27" s="65"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45" t="s">
+      <c r="B28" s="53"/>
+      <c r="C28" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="46"/>
-    </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="62" t="s">
+      <c r="D28" s="54"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63" t="s">
+      <c r="B29" s="45"/>
+      <c r="C29" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="69"/>
-    </row>
-    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="64" t="s">
+      <c r="D29" s="51"/>
+    </row>
+    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65" t="s">
+      <c r="B30" s="47"/>
+      <c r="C30" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="70"/>
-    </row>
-    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="62" t="s">
+      <c r="D30" s="52"/>
+    </row>
+    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63" t="s">
+      <c r="B31" s="45"/>
+      <c r="C31" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="69"/>
-    </row>
-    <row r="32" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="66" t="s">
+      <c r="D31" s="51"/>
+    </row>
+    <row r="32" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67" t="s">
+      <c r="B32" s="49"/>
+      <c r="C32" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="68"/>
+      <c r="D32" s="50"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="A31:B31"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:D23"/>
@@ -6675,16 +6507,24 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="I8:I14 D8:D18">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Planejamento da próxima semana
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 0310/Grupo4_ATA_Semana0310.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 0310/Grupo4_ATA_Semana0310.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\Semana 0310\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F54A0D-A5F4-4AEE-847A-2BE48897ACF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2BBAB7-B551-425E-BD84-B4CB115AD9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="7" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="70">
   <si>
     <t>NOME</t>
   </si>
@@ -150,9 +150,6 @@
     <t>PROTOTIPAÇÃO DO SITE</t>
   </si>
   <si>
-    <t>ALTERAÇÃO DAS TABELAS SQL</t>
-  </si>
-  <si>
     <t>DIAGRAMA DE SOLUÇÃO</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>MODELAGEM DE DADOS</t>
   </si>
   <si>
-    <t>INSTALAR O MYSQL na VM Local</t>
-  </si>
-  <si>
     <t>Sprint Review - Gasbusters (Grupo 4)</t>
   </si>
   <si>
@@ -256,6 +250,9 @@
   </si>
   <si>
     <t>Possivelmente saiu da faculdade</t>
+  </si>
+  <si>
+    <t>REVER O PROJETO TODO</t>
   </si>
 </sst>
 </file>
@@ -936,6 +933,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -961,57 +1009,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1348,6 +1345,103 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1484,107 +1578,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -3182,29 +3175,29 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D17" totalsRowShown="0" headerRowDxfId="45" tableBorderDxfId="44">
-  <autoFilter ref="A7:D17" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D14" totalsRowShown="0" headerRowDxfId="45" tableBorderDxfId="44">
+  <autoFilter ref="A7:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I14" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
-  <autoFilter ref="F7:I14" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I13" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
+  <autoFilter ref="F7:I13" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
     <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3683,7 +3676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440FA3E8-7F0D-4287-A3E8-76B61D68049B}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -3738,7 +3731,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="6">
         <v>45574</v>
@@ -3770,7 +3763,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="6">
         <v>45574</v>
@@ -3784,7 +3777,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="6">
         <v>45574</v>
@@ -3798,7 +3791,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="6">
         <v>45574</v>
@@ -3812,7 +3805,7 @@
     </row>
     <row r="10" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="6">
         <v>45574</v>
@@ -3826,7 +3819,7 @@
     </row>
     <row r="11" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="6">
         <v>45574</v>
@@ -3840,7 +3833,7 @@
     </row>
     <row r="12" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="6">
         <v>45574</v>
@@ -3863,7 +3856,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -4108,7 +4101,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4140,7 +4133,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6">
         <v>45565</v>
@@ -4168,7 +4161,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4210,7 +4203,7 @@
     </row>
     <row r="12" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6">
         <v>45572</v>
@@ -4224,7 +4217,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="6">
         <v>45573</v>
@@ -4238,7 +4231,7 @@
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" s="6">
         <v>45574</v>
@@ -4252,7 +4245,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="6">
         <v>45575</v>
@@ -4275,7 +4268,7 @@
     </row>
     <row r="18" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -4516,7 +4509,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4548,7 +4541,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6">
         <v>45565</v>
@@ -4576,7 +4569,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4618,7 +4611,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6">
         <v>45572</v>
@@ -4632,7 +4625,7 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="6">
         <v>45573</v>
@@ -4646,7 +4639,7 @@
     </row>
     <row r="14" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" s="6">
         <v>45574</v>
@@ -4660,7 +4653,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="6">
         <v>45575</v>
@@ -4688,7 +4681,7 @@
     </row>
     <row r="18" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -4932,7 +4925,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6">
         <v>45569</v>
@@ -4964,7 +4957,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="6">
         <v>45569</v>
@@ -4978,7 +4971,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="6">
         <v>45568</v>
@@ -4992,7 +4985,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -5034,7 +5027,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6">
         <v>45567</v>
@@ -5048,7 +5041,7 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="6">
         <v>45567</v>
@@ -5077,7 +5070,7 @@
     </row>
     <row r="17" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -5318,7 +5311,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6">
         <v>45575</v>
@@ -5350,7 +5343,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="6">
         <v>45575</v>
@@ -5364,7 +5357,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="6">
         <v>45575</v>
@@ -5378,7 +5371,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" s="6">
         <v>45572</v>
@@ -5420,7 +5413,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6">
         <v>45575</v>
@@ -5434,7 +5427,7 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="6">
         <v>45575</v>
@@ -5462,7 +5455,7 @@
     </row>
     <row r="16" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -5543,7 +5536,7 @@
         <v>15</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>22</v>
@@ -5653,7 +5646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA814AF-35E5-4596-923E-E8BF36EBF589}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:D18"/>
     </sheetView>
   </sheetViews>
@@ -5708,7 +5701,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6">
         <v>45575</v>
@@ -5726,7 +5719,7 @@
     </row>
     <row r="6" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="6">
         <v>45575</v>
@@ -5740,7 +5733,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="6">
         <v>45575</v>
@@ -5754,7 +5747,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="6">
         <v>45572</v>
@@ -5796,7 +5789,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6">
         <v>45575</v>
@@ -5810,7 +5803,7 @@
     </row>
     <row r="12" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B12" s="6">
         <v>45575</v>
@@ -5833,7 +5826,7 @@
     </row>
     <row r="15" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
@@ -5914,7 +5907,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>22</v>
@@ -5975,13 +5968,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D12">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6030,8 +6023,8 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:I14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6050,7 +6043,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -6070,7 +6063,7 @@
       <c r="C3" s="22"/>
       <c r="D3" s="23"/>
       <c r="F3" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
@@ -6080,37 +6073,37 @@
       <c r="A4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
+      <c r="B4" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="46"/>
+      <c r="D4" s="47"/>
       <c r="F4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
+      <c r="G4" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="46"/>
+      <c r="I4" s="47"/>
     </row>
     <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="58"/>
+      <c r="B5" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
       <c r="F5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
+      <c r="G5" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="48"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -6141,19 +6134,19 @@
     </row>
     <row r="8" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B8" s="6">
-        <v>45567</v>
+        <v>45574</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G8" s="6">
         <v>45574</v>
@@ -6167,13 +6160,13 @@
     </row>
     <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B9" s="6">
-        <v>45567</v>
+        <v>45574</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>17</v>
@@ -6193,19 +6186,19 @@
     </row>
     <row r="10" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="6">
-        <v>45567</v>
+        <v>45574</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="6">
         <v>45574</v>
@@ -6214,24 +6207,24 @@
         <v>10</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>27</v>
+      <c r="A11" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="B11" s="6">
-        <v>45567</v>
+        <v>45574</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G11" s="6">
         <v>45574</v>
@@ -6240,24 +6233,24 @@
         <v>12</v>
       </c>
       <c r="I11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45574</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="6">
-        <v>45567</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>16</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G12" s="6">
         <v>45574</v>
@@ -6270,20 +6263,20 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>35</v>
+      <c r="A13" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="B13" s="6">
-        <v>45567</v>
+        <v>45574</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="G13" s="6">
         <v>45574</v>
@@ -6296,204 +6289,161 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>34</v>
+      <c r="A14" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="B14" s="6">
-        <v>45567</v>
+        <v>45574</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="6">
-        <v>45574</v>
-      </c>
-      <c r="H14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="6">
-        <v>45567</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="6">
-        <v>45567</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>18</v>
-      </c>
+    <row r="15" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
     </row>
     <row r="17" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+    </row>
+    <row r="19" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
+    </row>
+    <row r="23" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="58"/>
+      <c r="C23" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="6">
-        <v>45567</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
-    </row>
-    <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-    </row>
-    <row r="21" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="30"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-    </row>
-    <row r="23" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="33"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="35"/>
-    </row>
-    <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="61"/>
-    </row>
-    <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="67"/>
+      <c r="D23" s="54"/>
+    </row>
+    <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="56"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="45"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="62"/>
       <c r="C26" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="63"/>
+        <v>42</v>
+      </c>
+      <c r="D26" s="68"/>
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="68" t="s">
-        <v>8</v>
+      <c r="A27" s="63" t="s">
+        <v>11</v>
       </c>
       <c r="B27" s="64"/>
       <c r="C27" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="65"/>
+        <v>43</v>
+      </c>
+      <c r="D27" s="69"/>
     </row>
     <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="54"/>
-    </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45" t="s">
+      <c r="A28" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="51"/>
-    </row>
-    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47" t="s">
+      <c r="D28" s="68"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="52"/>
-    </row>
-    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="51"/>
-    </row>
-    <row r="32" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="50"/>
-    </row>
+      <c r="D29" s="67"/>
+    </row>
+    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D23"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D20"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B4:D4"/>
@@ -6501,38 +6451,25 @@
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="F3:I3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I14 D8:D18">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="I8:I13 D8:D15">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B5" xr:uid="{2E14A627-A508-4036-9948-768B809E3863}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
   <tableParts count="2">
@@ -6546,13 +6483,13 @@
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D8:D18 I8:I14</xm:sqref>
+          <xm:sqref>I8:I13 D8:D15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CB2ECE66-384A-4231-9DE0-EE40A3A51602}">
           <x14:formula1>
             <xm:f>Quinta!$A$22:$A$27</xm:f>
           </x14:formula1>
-          <xm:sqref>G4:I5 H8:H14 C8:C18</xm:sqref>
+          <xm:sqref>B4:D5 H8:H13 G4:I5 C8:C15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>